<commit_message>
prepared code for aligned model on unaligned data and vice versa
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA00060-DBBF-4486-B4BD-79F87BF2611B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BAEEF5-E0F5-49E9-BBD2-BE8C9BC577EF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>Comparison of different CNN</t>
   </si>
@@ -161,11 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -482,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -595,57 +597,57 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30.6" x14ac:dyDescent="1.1000000000000001">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
+      <c r="B15" s="4">
+        <v>0.91017873999200005</v>
+      </c>
+      <c r="C15" s="4">
+        <v>8.8132549950699995E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>0.90420036555600003</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>8.9764793522200001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>0.87331375725399996</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>0.11655520891100001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>0.83986671568899995</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>0.12284109696499999</v>
       </c>
     </row>
@@ -694,14 +696,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>15</v>
+      <c r="B25" s="4">
+        <v>0.60563551777400004</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.28565417987199998</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
@@ -738,36 +740,36 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>15</v>
+      <c r="B34" s="4">
+        <v>0.93528623513599995</v>
+      </c>
+      <c r="C34" s="4">
+        <v>8.1481749141499998E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>15</v>
+      <c r="B35" s="4">
+        <v>0.91017873999200005</v>
+      </c>
+      <c r="C35" s="4">
+        <v>8.8132549950699995E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">

</xml_diff>

<commit_message>
delelted some stupid files...
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF38781E-6588-451C-810E-0F58DCC1B00B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0769AE36-C379-4636-99F5-01568E3CA2B7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Comparison of different CNN</t>
   </si>
@@ -84,13 +84,7 @@
     <t>Augmented vs. Unaugmented</t>
   </si>
   <si>
-    <t>Unaligned Augmented</t>
-  </si>
-  <si>
     <t>Unaligned Unaugmented</t>
-  </si>
-  <si>
-    <t>Aligned Augmented</t>
   </si>
   <si>
     <t>Aligned Unaugmented</t>
@@ -475,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -496,7 +490,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -600,7 +594,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4">
         <v>0.91017873999200005</v>
@@ -710,7 +704,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" s="4">
         <v>0.93528623513599995</v>
@@ -721,7 +715,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B30" s="4">
         <v>0.91017873999200005</v>
@@ -742,46 +736,46 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.60563551777400004</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.28565417987199998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0.90420036555600003</v>
+      </c>
+      <c r="C36" s="4">
+        <v>8.9764793522200001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new cropped run, batch size = 1
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4009AAB3-521E-4340-B82F-CF77F60DAC0F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287D1BBF-E4BD-4AFA-B966-B624535DB515}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Comparison of different CNN</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Aligned_CL9_DL1_nobias_200Epoch_0.0001LR1Batch1keep0WD</t>
+  </si>
+  <si>
+    <t>Aligned_cropped_CL9_DL1_nobias_200Epoch_0.0001LR1Batch1keep0WD</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -596,14 +599,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
+      <c r="B15" s="4">
+        <v>0.92198325694600003</v>
+      </c>
+      <c r="C15" s="4">
+        <v>8.0061481612300006E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -728,68 +731,95 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B32" s="4">
         <v>0.91017873999200005</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C32" s="4">
         <v>8.8132549950699995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
-      <c r="A34" s="5" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.92198325694600003</v>
+      </c>
+      <c r="C33" s="4">
+        <v>8.0061481612300006E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="36" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="4">
-        <v>0.60563551777400004</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0.28565417987199998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="4">
-        <v>0.75174814291600001</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0.20074279414900001</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B37" s="4">
-        <v>0.90420036555600003</v>
+        <v>0.60563551777400004</v>
       </c>
       <c r="C37" s="4">
-        <v>8.9764793522200001E-2</v>
+        <v>0.28565417987199998</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.75174814291600001</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.20074279414900001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.90420036555600003</v>
+      </c>
+      <c r="C39" s="4">
+        <v>8.9764793522200001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B40" s="4">
         <v>0.80385281586099999</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C40" s="4">
         <v>0.162580160645</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed batch size for aligned data
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287D1BBF-E4BD-4AFA-B966-B624535DB515}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8131D687-9ED4-4928-9BA5-D4780C47A8A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Comparison of different CNN</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Aligned_cropped_CL9_DL1_nobias_200Epoch_0.0001LR1Batch1keep0WD</t>
+  </si>
+  <si>
+    <t>MSE:</t>
   </si>
 </sst>
 </file>
@@ -475,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -494,6 +497,9 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="3" t="s">
         <v>22</v>
@@ -531,6 +537,9 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -597,6 +606,9 @@
       <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
@@ -620,7 +632,7 @@
         <v>8.8132549950699995E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -631,7 +643,7 @@
         <v>8.9764793522200001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -642,7 +654,7 @@
         <v>0.11655520891100001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -653,7 +665,7 @@
         <v>0.12284109696499999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="22" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -663,8 +675,11 @@
       <c r="C22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -675,7 +690,7 @@
         <v>0.10076319081399999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -686,7 +701,7 @@
         <v>8.9764793522200001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -697,7 +712,7 @@
         <v>0.26574004318599997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -708,7 +723,7 @@
         <v>0.28565417987199998</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="29" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
@@ -718,8 +733,11 @@
       <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -730,7 +748,7 @@
         <v>8.1481749141499998E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
@@ -741,7 +759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
@@ -752,7 +770,7 @@
         <v>8.8132549950699995E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4" t="s">
         <v>24</v>
       </c>
@@ -763,12 +781,12 @@
         <v>8.0061481612300006E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="36" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A36" s="5" t="s">
         <v>18</v>
       </c>
@@ -778,8 +796,11 @@
       <c r="C36" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
         <v>14</v>
       </c>
@@ -790,7 +811,7 @@
         <v>0.28565417987199998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
         <v>19</v>
       </c>
@@ -801,7 +822,7 @@
         <v>0.20074279414900001</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
@@ -812,7 +833,7 @@
         <v>8.9764793522200001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
changed batch size to 16
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8131D687-9ED4-4928-9BA5-D4780C47A8A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEBEF24-EDF7-4991-AF50-D5BF3CFB5686}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -620,6 +620,9 @@
       <c r="C15" s="4">
         <v>8.0061481612300006E-2</v>
       </c>
+      <c r="D15">
+        <v>1032.94294633</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
@@ -631,6 +634,9 @@
       <c r="C16" s="4">
         <v>8.8132549950699995E-2</v>
       </c>
+      <c r="D16">
+        <v>1095.0160229200001</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
@@ -722,6 +728,9 @@
       <c r="C26" s="4">
         <v>0.28565417987199998</v>
       </c>
+      <c r="D26">
+        <v>10669.743807999999</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A29" s="5" t="s">
@@ -769,6 +778,9 @@
       <c r="C32" s="4">
         <v>8.8132549950699995E-2</v>
       </c>
+      <c r="D32">
+        <v>1095.0160229200001</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4" t="s">
@@ -779,6 +791,9 @@
       </c>
       <c r="C33" s="4">
         <v>8.0061481612300006E-2</v>
+      </c>
+      <c r="D33">
+        <v>1032.94294633</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -809,6 +824,9 @@
       </c>
       <c r="C37" s="4">
         <v>0.28565417987199998</v>
+      </c>
+      <c r="D37">
+        <v>10669.743807999999</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
changed batch-size to 64
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058B0DB2-D241-44AB-B3FE-8A199613A541}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A39E9F3-8F5B-410E-847B-9A4C36EAD589}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -584,6 +584,9 @@
       <c r="C10">
         <v>8.9764793522200001E-2</v>
       </c>
+      <c r="D10">
+        <v>1131.9497092199999</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
@@ -648,6 +651,9 @@
       <c r="C17" s="4">
         <v>8.9764793522200001E-2</v>
       </c>
+      <c r="D17">
+        <v>1131.9497092199999</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
@@ -705,6 +711,9 @@
       </c>
       <c r="C24">
         <v>8.9764793522200001E-2</v>
+      </c>
+      <c r="D24">
+        <v>1131.9497092199999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -849,6 +858,9 @@
       </c>
       <c r="C39" s="4">
         <v>8.9764793522200001E-2</v>
+      </c>
+      <c r="D39">
+        <v>1131.9497092199999</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
changed batch size to 1 (best result!)
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\3D-Vision-Project\Prediction_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A39E9F3-8F5B-410E-847B-9A4C36EAD589}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12380188-F52C-49E6-87DD-CECCB77540A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{AC8906FB-054F-4932-B2AE-6F24746D1AAB}"/>
   </bookViews>
@@ -84,12 +84,6 @@
     <t>Augmented vs. Unaugmented</t>
   </si>
   <si>
-    <t>Unaligned Unaugmented</t>
-  </si>
-  <si>
-    <t>Aligned Unaugmented</t>
-  </si>
-  <si>
     <t>Aligned_CL9_DL1_nobias_200Epoch_0.0001LR3Batch1keep0WD</t>
   </si>
   <si>
@@ -106,6 +100,12 @@
   </si>
   <si>
     <t>MSE:</t>
+  </si>
+  <si>
+    <t>Unaligned_unaug_CL9_DL1_nobias_200Epoch_0.0001LR5Batch1keep0WD</t>
+  </si>
+  <si>
+    <t>Aligned_unaug_CL9_DL1_nobias_200Epoch_0.0001LR5Batch1keep0WD</t>
   </si>
 </sst>
 </file>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFA2C80-8683-489D-8E09-70F132598910}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -498,11 +498,11 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -538,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -610,12 +610,12 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4">
         <v>0.92198325694600003</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="4">
         <v>0.91017873999200005</v>
@@ -665,6 +665,9 @@
       <c r="C18" s="4">
         <v>0.11655520891100001</v>
       </c>
+      <c r="D18">
+        <v>1482.06628226</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
@@ -688,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -752,12 +755,12 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B30" s="4">
         <v>0.93528623513599995</v>
@@ -768,7 +771,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>15</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B32" s="4">
         <v>0.91017873999200005</v>
@@ -793,7 +796,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" s="4">
         <v>0.92198325694600003</v>
@@ -821,7 +824,7 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -840,7 +843,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B38" s="4">
         <v>0.75174814291600001</v>
@@ -865,7 +868,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B40" s="4">
         <v>0.80385281586099999</v>

</xml_diff>

<commit_message>
new readme and updated results-file in excel
</commit_message>
<xml_diff>
--- a/Prediction_Data/Results.xlsx
+++ b/Prediction_Data/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Dropbox\3D Vision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52CFAC8-7715-474E-8D44-AB39967A49E0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBD3F23-0FBE-4503-A5CD-E34E02972163}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16386" windowHeight="8190" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Aligned vs. Unaligned</t>
   </si>
@@ -495,20 +495,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.89453125" style="2"/>
-    <col min="2" max="1025" width="12.3671875" style="2"/>
-    <col min="1026" max="16384" width="8.83984375" style="2"/>
+    <col min="1" max="1" width="70.85546875" style="2"/>
+    <col min="2" max="1025" width="12.42578125" style="2"/>
+    <col min="1026" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -536,7 +536,7 @@
         <v>1592.96645532</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -550,7 +550,7 @@
         <v>12795.504245300001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -564,7 +564,7 @@
         <v>1127.5681931300001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -578,7 +578,7 @@
         <v>11134.274969300001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -592,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -606,7 +606,7 @@
         <v>1330.44086008</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -620,7 +620,7 @@
         <v>1309.73148165</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -634,7 +634,7 @@
         <v>1127.5681931300001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -648,7 +648,7 @@
         <v>1131.9497092199999</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -662,7 +662,7 @@
         <v>4605.7295162999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -676,7 +676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1032.94294633</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -704,7 +704,7 @@
         <v>1095.0160229200001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -718,7 +718,7 @@
         <v>1131.9497092199999</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -732,7 +732,7 @@
         <v>1482.06628226</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -746,7 +746,7 @@
         <v>1875.98949399</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -760,7 +760,7 @@
         <v>1127.5681931300001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -774,7 +774,7 @@
         <v>1011.83499377</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="28" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -788,7 +788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>4</v>
       </c>
@@ -802,7 +802,7 @@
         <v>1592.96645532</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -816,7 +816,7 @@
         <v>1131.9497092199999</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
@@ -830,7 +830,7 @@
         <v>12795.504245300001</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -844,7 +844,7 @@
         <v>10669.743807999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -858,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>22</v>
       </c>
@@ -872,7 +872,7 @@
         <v>931.36019090399998</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>23</v>
       </c>
@@ -886,7 +886,7 @@
         <v>914.58856762999994</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -900,7 +900,7 @@
         <v>1095.0160229200001</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -914,7 +914,7 @@
         <v>1032.94294633</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>24</v>
       </c>
@@ -928,171 +928,185 @@
         <v>918.85495743299998</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
-      <c r="A43" s="1" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.92467501381299999</v>
+      </c>
+      <c r="C42" s="2">
+        <v>7.7470288397699996E-2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1011.83499377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B45" s="2">
         <v>0.60563551777400004</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C45" s="2">
         <v>0.28565417987199998</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D45" s="2">
         <v>10669.743807999999</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B46" s="2">
         <v>0.75174814291600001</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C46" s="2">
         <v>0.20074279414900001</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D46" s="2">
         <v>3665.72620843</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B47" s="2">
         <v>0.90420036555600003</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C47" s="2">
         <v>8.9764793522200001E-2</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D47" s="2">
         <v>1131.9497092199999</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B48" s="2">
         <v>0.80385281586099999</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C48" s="2">
         <v>0.162580160645</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D48" s="2">
         <v>2378.4653884999998</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B50" s="2">
         <v>0.90305176214299998</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C50" s="2">
         <v>9.2769244860699998E-2</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D50" s="2">
         <v>1127.5681931300001</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B51" s="3">
         <v>0.73296481079999998</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C51" s="3">
         <v>0.20711502660700001</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D51" s="3">
         <v>4067.5784216500001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B52" s="3">
         <v>0.82450739447900001</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C52" s="3">
         <v>0.144788263606</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D52" s="3">
         <v>2150.7607392199998</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="3" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B53" s="2">
         <v>0.60256947306700004</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C53" s="2">
         <v>0.28037471741199999</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D53" s="2">
         <v>11134.274969300001</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30.6" x14ac:dyDescent="1.1000000000000001">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A56" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B57" s="2">
         <v>0.33527098049499998</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C57" s="2">
         <v>0.33733773382100002</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D57" s="2">
         <v>74246.395034400004</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B58" s="2">
         <v>0.25786639009099999</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C58" s="2">
         <v>0.32640203636699999</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D58" s="2">
         <v>98983.513007300004</v>
       </c>
     </row>

</xml_diff>